<commit_message>
Fixed small error in BOM
</commit_message>
<xml_diff>
--- a/resources/Add-ons/linear_input/BOM.xlsx
+++ b/resources/Add-ons/linear_input/BOM.xlsx
@@ -55,7 +55,7 @@
     <t>R3, R4</t>
   </si>
   <si>
-    <t>4.7kOhm</t>
+    <t>1mOhm</t>
   </si>
   <si>
     <t>S1MQCT-ND</t>
@@ -162,7 +162,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -312,13 +312,75 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -360,6 +422,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1448,7 +1528,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1603,6 +1683,22 @@
         <v>1</v>
       </c>
     </row>
+    <row r="9" ht="14.7" customHeight="1">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="16"/>
+    </row>
+    <row r="10" ht="14.7" customHeight="1">
+      <c r="A10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="19"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>

</xml_diff>